<commit_message>
Discretização de todas variáveis, nova árvore de decisão e código do chatbot
</commit_message>
<xml_diff>
--- a/Dados/casas_98058.xlsx
+++ b/Dados/casas_98058.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">price</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">preco_area_construida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zipcode</t>
   </si>
 </sst>
 </file>
@@ -170,10 +173,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1000"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -185,7 +188,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="7.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.91"/>
@@ -239,6 +242,9 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -283,6 +289,9 @@
       <c r="N2" s="1" t="n">
         <v>156.5533981</v>
       </c>
+      <c r="O2" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -327,6 +336,9 @@
       <c r="N3" s="1" t="n">
         <v>241.40625</v>
       </c>
+      <c r="O3" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -371,6 +383,9 @@
       <c r="N4" s="1" t="n">
         <v>239.6694215</v>
       </c>
+      <c r="O4" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -415,6 +430,9 @@
       <c r="N5" s="1" t="n">
         <v>160.2564103</v>
       </c>
+      <c r="O5" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -459,6 +477,9 @@
       <c r="N6" s="1" t="n">
         <v>127.3291925</v>
       </c>
+      <c r="O6" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -503,6 +524,9 @@
       <c r="N7" s="1" t="n">
         <v>182.2033898</v>
       </c>
+      <c r="O7" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -547,6 +571,9 @@
       <c r="N8" s="1" t="n">
         <v>140.2941176</v>
       </c>
+      <c r="O8" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -591,6 +618,9 @@
       <c r="N9" s="1" t="n">
         <v>135.4166667</v>
       </c>
+      <c r="O9" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -635,6 +665,9 @@
       <c r="N10" s="1" t="n">
         <v>196.5065502</v>
       </c>
+      <c r="O10" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -679,6 +712,9 @@
       <c r="N11" s="1" t="n">
         <v>156.4102564</v>
       </c>
+      <c r="O11" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -723,6 +759,9 @@
       <c r="N12" s="1" t="n">
         <v>152.9393939</v>
       </c>
+      <c r="O12" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -767,6 +806,9 @@
       <c r="N13" s="1" t="n">
         <v>176.4052288</v>
       </c>
+      <c r="O13" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -811,6 +853,9 @@
       <c r="N14" s="1" t="n">
         <v>166.6666667</v>
       </c>
+      <c r="O14" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -855,6 +900,9 @@
       <c r="N15" s="1" t="n">
         <v>165.9090909</v>
       </c>
+      <c r="O15" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -899,6 +947,9 @@
       <c r="N16" s="1" t="n">
         <v>242.0168067</v>
       </c>
+      <c r="O16" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -943,6 +994,9 @@
       <c r="N17" s="1" t="n">
         <v>222.3602484</v>
       </c>
+      <c r="O17" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -987,6 +1041,9 @@
       <c r="N18" s="1" t="n">
         <v>136.9565217</v>
       </c>
+      <c r="O18" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1031,6 +1088,9 @@
       <c r="N19" s="1" t="n">
         <v>198.1203008</v>
       </c>
+      <c r="O19" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -1075,6 +1135,9 @@
       <c r="N20" s="1" t="n">
         <v>213.8888889</v>
       </c>
+      <c r="O20" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -1119,6 +1182,9 @@
       <c r="N21" s="1" t="n">
         <v>145.708502</v>
       </c>
+      <c r="O21" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -1163,6 +1229,9 @@
       <c r="N22" s="1" t="n">
         <v>193.9393939</v>
       </c>
+      <c r="O22" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -1207,6 +1276,9 @@
       <c r="N23" s="1" t="n">
         <v>176.3285024</v>
       </c>
+      <c r="O23" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -1251,6 +1323,9 @@
       <c r="N24" s="1" t="n">
         <v>162.8409091</v>
       </c>
+      <c r="O24" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -1295,6 +1370,9 @@
       <c r="N25" s="1" t="n">
         <v>196.6292135</v>
       </c>
+      <c r="O25" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -1339,6 +1417,9 @@
       <c r="N26" s="1" t="n">
         <v>202.7027027</v>
       </c>
+      <c r="O26" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -1383,6 +1464,9 @@
       <c r="N27" s="1" t="n">
         <v>136.7924528</v>
       </c>
+      <c r="O27" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -1427,6 +1511,9 @@
       <c r="N28" s="1" t="n">
         <v>151.7509728</v>
       </c>
+      <c r="O28" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -1471,6 +1558,9 @@
       <c r="N29" s="1" t="n">
         <v>173.0769231</v>
       </c>
+      <c r="O29" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -1515,6 +1605,9 @@
       <c r="N30" s="1" t="n">
         <v>146.627566</v>
       </c>
+      <c r="O30" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -1559,6 +1652,9 @@
       <c r="N31" s="1" t="n">
         <v>156.5972222</v>
       </c>
+      <c r="O31" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
@@ -1603,6 +1699,9 @@
       <c r="N32" s="1" t="n">
         <v>206.7592593</v>
       </c>
+      <c r="O32" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -1647,6 +1746,9 @@
       <c r="N33" s="1" t="n">
         <v>109.7852029</v>
       </c>
+      <c r="O33" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
@@ -1691,6 +1793,9 @@
       <c r="N34" s="1" t="n">
         <v>180.1136364</v>
       </c>
+      <c r="O34" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -1735,6 +1840,9 @@
       <c r="N35" s="1" t="n">
         <v>245.8333333</v>
       </c>
+      <c r="O35" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
@@ -1779,6 +1887,9 @@
       <c r="N36" s="1" t="n">
         <v>217.7419355</v>
       </c>
+      <c r="O36" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -1823,6 +1934,9 @@
       <c r="N37" s="1" t="n">
         <v>157.2448276</v>
       </c>
+      <c r="O37" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
@@ -1867,6 +1981,9 @@
       <c r="N38" s="1" t="n">
         <v>202.5316456</v>
       </c>
+      <c r="O38" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -1911,6 +2028,9 @@
       <c r="N39" s="1" t="n">
         <v>141.7004049</v>
       </c>
+      <c r="O39" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -1955,6 +2075,9 @@
       <c r="N40" s="1" t="n">
         <v>216.1016949</v>
       </c>
+      <c r="O40" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
@@ -1999,6 +2122,9 @@
       <c r="N41" s="1" t="n">
         <v>159.3406593</v>
       </c>
+      <c r="O41" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -2043,6 +2169,9 @@
       <c r="N42" s="1" t="n">
         <v>182.7411168</v>
       </c>
+      <c r="O42" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -2087,6 +2216,9 @@
       <c r="N43" s="1" t="n">
         <v>295.4545455</v>
       </c>
+      <c r="O43" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
@@ -2131,6 +2263,9 @@
       <c r="N44" s="1" t="n">
         <v>183.4170854</v>
       </c>
+      <c r="O44" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -2175,6 +2310,9 @@
       <c r="N45" s="1" t="n">
         <v>136.3636364</v>
       </c>
+      <c r="O45" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
@@ -2219,6 +2357,9 @@
       <c r="N46" s="1" t="n">
         <v>164.2857143</v>
       </c>
+      <c r="O46" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
@@ -2263,6 +2404,9 @@
       <c r="N47" s="1" t="n">
         <v>194.9838188</v>
       </c>
+      <c r="O47" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -2307,6 +2451,9 @@
       <c r="N48" s="1" t="n">
         <v>117.2077922</v>
       </c>
+      <c r="O48" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
@@ -2351,6 +2498,9 @@
       <c r="N49" s="1" t="n">
         <v>162.2009569</v>
       </c>
+      <c r="O49" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
@@ -2395,6 +2545,9 @@
       <c r="N50" s="1" t="n">
         <v>167.3819742</v>
       </c>
+      <c r="O50" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
@@ -2439,6 +2592,9 @@
       <c r="N51" s="1" t="n">
         <v>185.0282486</v>
       </c>
+      <c r="O51" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
@@ -2483,6 +2639,9 @@
       <c r="N52" s="1" t="n">
         <v>133.492823</v>
       </c>
+      <c r="O52" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
@@ -2527,6 +2686,9 @@
       <c r="N53" s="1" t="n">
         <v>126.9230769</v>
       </c>
+      <c r="O53" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
@@ -2571,6 +2733,9 @@
       <c r="N54" s="1" t="n">
         <v>206.5217391</v>
       </c>
+      <c r="O54" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
@@ -2615,6 +2780,9 @@
       <c r="N55" s="1" t="n">
         <v>200.8522727</v>
       </c>
+      <c r="O55" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
@@ -2659,6 +2827,9 @@
       <c r="N56" s="1" t="n">
         <v>174.2248062</v>
       </c>
+      <c r="O56" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
@@ -2703,6 +2874,9 @@
       <c r="N57" s="1" t="n">
         <v>220.3389831</v>
       </c>
+      <c r="O57" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
@@ -2747,6 +2921,9 @@
       <c r="N58" s="1" t="n">
         <v>197.3856209</v>
       </c>
+      <c r="O58" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
@@ -2791,6 +2968,9 @@
       <c r="N59" s="1" t="n">
         <v>155.9485531</v>
       </c>
+      <c r="O59" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
@@ -2835,6 +3015,9 @@
       <c r="N60" s="1" t="n">
         <v>236.9158879</v>
       </c>
+      <c r="O60" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
@@ -2879,6 +3062,9 @@
       <c r="N61" s="1" t="n">
         <v>145.4545455</v>
       </c>
+      <c r="O61" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
@@ -2923,6 +3109,9 @@
       <c r="N62" s="1" t="n">
         <v>171.5083799</v>
       </c>
+      <c r="O62" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
@@ -2967,6 +3156,9 @@
       <c r="N63" s="1" t="n">
         <v>112.9707113</v>
       </c>
+      <c r="O63" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
@@ -3011,6 +3203,9 @@
       <c r="N64" s="1" t="n">
         <v>190.3914591</v>
       </c>
+      <c r="O64" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
@@ -3055,6 +3250,9 @@
       <c r="N65" s="1" t="n">
         <v>129.2682927</v>
       </c>
+      <c r="O65" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
@@ -3099,6 +3297,9 @@
       <c r="N66" s="1" t="n">
         <v>164.8241206</v>
       </c>
+      <c r="O66" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
@@ -3143,6 +3344,9 @@
       <c r="N67" s="1" t="n">
         <v>172.5581395</v>
       </c>
+      <c r="O67" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
@@ -3187,6 +3391,9 @@
       <c r="N68" s="1" t="n">
         <v>176.1006289</v>
       </c>
+      <c r="O68" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
@@ -3231,6 +3438,9 @@
       <c r="N69" s="1" t="n">
         <v>203.3898305</v>
       </c>
+      <c r="O69" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
@@ -3275,6 +3485,9 @@
       <c r="N70" s="1" t="n">
         <v>188.121547</v>
       </c>
+      <c r="O70" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
@@ -3319,6 +3532,9 @@
       <c r="N71" s="1" t="n">
         <v>151.7467249</v>
       </c>
+      <c r="O71" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
@@ -3363,6 +3579,9 @@
       <c r="N72" s="1" t="n">
         <v>242.1052632</v>
       </c>
+      <c r="O72" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
@@ -3407,6 +3626,9 @@
       <c r="N73" s="1" t="n">
         <v>133.1707317</v>
       </c>
+      <c r="O73" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
@@ -3451,6 +3673,9 @@
       <c r="N74" s="1" t="n">
         <v>180.8441558</v>
       </c>
+      <c r="O74" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
@@ -3495,6 +3720,9 @@
       <c r="N75" s="1" t="n">
         <v>154.5801527</v>
       </c>
+      <c r="O75" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
@@ -3539,6 +3767,9 @@
       <c r="N76" s="1" t="n">
         <v>140.5109489</v>
       </c>
+      <c r="O76" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
@@ -3583,6 +3814,9 @@
       <c r="N77" s="1" t="n">
         <v>124.4444444</v>
       </c>
+      <c r="O77" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
@@ -3627,6 +3861,9 @@
       <c r="N78" s="1" t="n">
         <v>177.6041667</v>
       </c>
+      <c r="O78" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
@@ -3671,6 +3908,9 @@
       <c r="N79" s="1" t="n">
         <v>229.0076336</v>
       </c>
+      <c r="O79" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
@@ -3715,6 +3955,9 @@
       <c r="N80" s="1" t="n">
         <v>178.9325843</v>
       </c>
+      <c r="O80" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
@@ -3759,6 +4002,9 @@
       <c r="N81" s="1" t="n">
         <v>172.7642276</v>
       </c>
+      <c r="O81" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
@@ -3803,6 +4049,9 @@
       <c r="N82" s="1" t="n">
         <v>144.4444444</v>
       </c>
+      <c r="O82" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
@@ -3847,6 +4096,9 @@
       <c r="N83" s="1" t="n">
         <v>143.1654676</v>
       </c>
+      <c r="O83" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
@@ -3891,6 +4143,9 @@
       <c r="N84" s="1" t="n">
         <v>253.2051282</v>
       </c>
+      <c r="O84" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
@@ -3935,6 +4190,9 @@
       <c r="N85" s="1" t="n">
         <v>208.3333333</v>
       </c>
+      <c r="O85" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
@@ -3979,6 +4237,9 @@
       <c r="N86" s="1" t="n">
         <v>129</v>
       </c>
+      <c r="O86" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
@@ -4023,6 +4284,9 @@
       <c r="N87" s="1" t="n">
         <v>168.4782609</v>
       </c>
+      <c r="O87" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
@@ -4067,6 +4331,9 @@
       <c r="N88" s="1" t="n">
         <v>136.3636364</v>
       </c>
+      <c r="O88" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
@@ -4111,6 +4378,9 @@
       <c r="N89" s="1" t="n">
         <v>371.9806763</v>
       </c>
+      <c r="O89" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
@@ -4155,6 +4425,9 @@
       <c r="N90" s="1" t="n">
         <v>139.8963731</v>
       </c>
+      <c r="O90" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
@@ -4199,6 +4472,9 @@
       <c r="N91" s="1" t="n">
         <v>142.5</v>
       </c>
+      <c r="O91" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
@@ -4243,6 +4519,9 @@
       <c r="N92" s="1" t="n">
         <v>209.7315436</v>
       </c>
+      <c r="O92" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="n">
@@ -4287,6 +4566,9 @@
       <c r="N93" s="1" t="n">
         <v>214.556962</v>
       </c>
+      <c r="O93" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="n">
@@ -4331,6 +4613,9 @@
       <c r="N94" s="1" t="n">
         <v>264.7214854</v>
       </c>
+      <c r="O94" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
@@ -4375,6 +4660,9 @@
       <c r="N95" s="1" t="n">
         <v>160.944206</v>
       </c>
+      <c r="O95" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
@@ -4419,6 +4707,9 @@
       <c r="N96" s="1" t="n">
         <v>191.2280702</v>
       </c>
+      <c r="O96" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
@@ -4463,6 +4754,9 @@
       <c r="N97" s="1" t="n">
         <v>198.081761</v>
       </c>
+      <c r="O97" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="n">
@@ -4507,6 +4801,9 @@
       <c r="N98" s="1" t="n">
         <v>146.9183673</v>
       </c>
+      <c r="O98" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="n">
@@ -4551,6 +4848,9 @@
       <c r="N99" s="1" t="n">
         <v>177.1043771</v>
       </c>
+      <c r="O99" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="n">
@@ -4595,6 +4895,9 @@
       <c r="N100" s="1" t="n">
         <v>166.6666667</v>
       </c>
+      <c r="O100" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="n">
@@ -4639,6 +4942,9 @@
       <c r="N101" s="1" t="n">
         <v>171.5346535</v>
       </c>
+      <c r="O101" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="n">
@@ -4683,6 +4989,9 @@
       <c r="N102" s="1" t="n">
         <v>167.3387097</v>
       </c>
+      <c r="O102" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="n">
@@ -4727,6 +5036,9 @@
       <c r="N103" s="1" t="n">
         <v>194.8571429</v>
       </c>
+      <c r="O103" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="n">
@@ -4771,6 +5083,9 @@
       <c r="N104" s="1" t="n">
         <v>215.7534247</v>
       </c>
+      <c r="O104" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="n">
@@ -4815,6 +5130,9 @@
       <c r="N105" s="1" t="n">
         <v>212.7304965</v>
       </c>
+      <c r="O105" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="n">
@@ -4859,6 +5177,9 @@
       <c r="N106" s="1" t="n">
         <v>122.605364</v>
       </c>
+      <c r="O106" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="n">
@@ -4903,6 +5224,9 @@
       <c r="N107" s="1" t="n">
         <v>229.3119266</v>
       </c>
+      <c r="O107" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="n">
@@ -4947,6 +5271,9 @@
       <c r="N108" s="1" t="n">
         <v>210.0006667</v>
       </c>
+      <c r="O108" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="n">
@@ -4991,6 +5318,9 @@
       <c r="N109" s="1" t="n">
         <v>163.9053254</v>
       </c>
+      <c r="O109" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="n">
@@ -5035,6 +5365,9 @@
       <c r="N110" s="1" t="n">
         <v>185.6785714</v>
       </c>
+      <c r="O110" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="n">
@@ -5079,6 +5412,9 @@
       <c r="N111" s="1" t="n">
         <v>210.4</v>
       </c>
+      <c r="O111" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="n">
@@ -5123,6 +5459,9 @@
       <c r="N112" s="1" t="n">
         <v>153.5545024</v>
       </c>
+      <c r="O112" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="n">
@@ -5167,6 +5506,9 @@
       <c r="N113" s="1" t="n">
         <v>149.7584541</v>
       </c>
+      <c r="O113" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="n">
@@ -5211,6 +5553,9 @@
       <c r="N114" s="1" t="n">
         <v>157.7380952</v>
       </c>
+      <c r="O114" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="n">
@@ -5255,6 +5600,9 @@
       <c r="N115" s="1" t="n">
         <v>165.9090909</v>
       </c>
+      <c r="O115" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
@@ -5299,6 +5647,9 @@
       <c r="N116" s="1" t="n">
         <v>203.0508475</v>
       </c>
+      <c r="O116" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="n">
@@ -5343,6 +5694,9 @@
       <c r="N117" s="1" t="n">
         <v>150.7936508</v>
       </c>
+      <c r="O117" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="n">
@@ -5387,6 +5741,9 @@
       <c r="N118" s="1" t="n">
         <v>184.6153846</v>
       </c>
+      <c r="O118" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="n">
@@ -5431,6 +5788,9 @@
       <c r="N119" s="1" t="n">
         <v>229.1666667</v>
       </c>
+      <c r="O119" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="n">
@@ -5475,6 +5835,9 @@
       <c r="N120" s="1" t="n">
         <v>178.5714286</v>
       </c>
+      <c r="O120" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="n">
@@ -5519,6 +5882,9 @@
       <c r="N121" s="1" t="n">
         <v>204.2253521</v>
       </c>
+      <c r="O121" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="n">
@@ -5563,6 +5929,9 @@
       <c r="N122" s="1" t="n">
         <v>181.122449</v>
       </c>
+      <c r="O122" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="n">
@@ -5607,6 +5976,9 @@
       <c r="N123" s="1" t="n">
         <v>186.9565217</v>
       </c>
+      <c r="O123" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="n">
@@ -5651,6 +6023,9 @@
       <c r="N124" s="1" t="n">
         <v>182.9738562</v>
       </c>
+      <c r="O124" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="n">
@@ -5695,6 +6070,9 @@
       <c r="N125" s="1" t="n">
         <v>159.0454545</v>
       </c>
+      <c r="O125" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="n">
@@ -5739,6 +6117,9 @@
       <c r="N126" s="1" t="n">
         <v>135.1706037</v>
       </c>
+      <c r="O126" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="n">
@@ -5783,6 +6164,9 @@
       <c r="N127" s="1" t="n">
         <v>103.125</v>
       </c>
+      <c r="O127" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="n">
@@ -5827,6 +6211,9 @@
       <c r="N128" s="1" t="n">
         <v>136.3636364</v>
       </c>
+      <c r="O128" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="n">
@@ -5871,6 +6258,9 @@
       <c r="N129" s="1" t="n">
         <v>180.0492611</v>
       </c>
+      <c r="O129" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="n">
@@ -5915,6 +6305,9 @@
       <c r="N130" s="1" t="n">
         <v>139.0243902</v>
       </c>
+      <c r="O130" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="n">
@@ -5959,6 +6352,9 @@
       <c r="N131" s="1" t="n">
         <v>232.9376855</v>
       </c>
+      <c r="O131" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="n">
@@ -6003,6 +6399,9 @@
       <c r="N132" s="1" t="n">
         <v>179.5774648</v>
       </c>
+      <c r="O132" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="n">
@@ -6047,6 +6446,9 @@
       <c r="N133" s="1" t="n">
         <v>167.9558011</v>
       </c>
+      <c r="O133" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="n">
@@ -6091,6 +6493,9 @@
       <c r="N134" s="1" t="n">
         <v>157.962963</v>
       </c>
+      <c r="O134" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="n">
@@ -6135,6 +6540,9 @@
       <c r="N135" s="1" t="n">
         <v>174.2424242</v>
       </c>
+      <c r="O135" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="n">
@@ -6179,6 +6587,9 @@
       <c r="N136" s="1" t="n">
         <v>185.6115108</v>
       </c>
+      <c r="O136" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="n">
@@ -6223,6 +6634,9 @@
       <c r="N137" s="1" t="n">
         <v>216.3716814</v>
       </c>
+      <c r="O137" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="n">
@@ -6267,6 +6681,9 @@
       <c r="N138" s="1" t="n">
         <v>167.4401914</v>
       </c>
+      <c r="O138" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="n">
@@ -6311,6 +6728,9 @@
       <c r="N139" s="1" t="n">
         <v>213.7586207</v>
       </c>
+      <c r="O139" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="n">
@@ -6355,6 +6775,9 @@
       <c r="N140" s="1" t="n">
         <v>198.4848485</v>
       </c>
+      <c r="O140" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="n">
@@ -6399,6 +6822,9 @@
       <c r="N141" s="1" t="n">
         <v>176.6917293</v>
       </c>
+      <c r="O141" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="n">
@@ -6443,6 +6869,9 @@
       <c r="N142" s="1" t="n">
         <v>121.7391304</v>
       </c>
+      <c r="O142" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="n">
@@ -6487,6 +6916,9 @@
       <c r="N143" s="1" t="n">
         <v>152.4064171</v>
       </c>
+      <c r="O143" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="n">
@@ -6531,6 +6963,9 @@
       <c r="N144" s="1" t="n">
         <v>160.9489051</v>
       </c>
+      <c r="O144" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="n">
@@ -6575,6 +7010,9 @@
       <c r="N145" s="1" t="n">
         <v>152.8089888</v>
       </c>
+      <c r="O145" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="n">
@@ -6619,6 +7057,9 @@
       <c r="N146" s="1" t="n">
         <v>170.212766</v>
       </c>
+      <c r="O146" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="n">
@@ -6663,6 +7104,9 @@
       <c r="N147" s="1" t="n">
         <v>211.4516129</v>
       </c>
+      <c r="O147" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="n">
@@ -6707,6 +7151,9 @@
       <c r="N148" s="1" t="n">
         <v>168.5393258</v>
       </c>
+      <c r="O148" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="n">
@@ -6751,6 +7198,9 @@
       <c r="N149" s="1" t="n">
         <v>165.7458564</v>
       </c>
+      <c r="O149" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="n">
@@ -6795,6 +7245,9 @@
       <c r="N150" s="1" t="n">
         <v>136.71875</v>
       </c>
+      <c r="O150" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="n">
@@ -6839,6 +7292,9 @@
       <c r="N151" s="1" t="n">
         <v>146.7005076</v>
       </c>
+      <c r="O151" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="n">
@@ -6883,6 +7339,9 @@
       <c r="N152" s="1" t="n">
         <v>165.8959538</v>
       </c>
+      <c r="O152" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="n">
@@ -6927,6 +7386,9 @@
       <c r="N153" s="1" t="n">
         <v>138.2575758</v>
       </c>
+      <c r="O153" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="n">
@@ -6971,6 +7433,9 @@
       <c r="N154" s="1" t="n">
         <v>115.2</v>
       </c>
+      <c r="O154" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="n">
@@ -7015,6 +7480,9 @@
       <c r="N155" s="1" t="n">
         <v>178.9473684</v>
       </c>
+      <c r="O155" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="n">
@@ -7059,6 +7527,9 @@
       <c r="N156" s="1" t="n">
         <v>140.8934708</v>
       </c>
+      <c r="O156" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="n">
@@ -7103,6 +7574,9 @@
       <c r="N157" s="1" t="n">
         <v>160.7142857</v>
       </c>
+      <c r="O157" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="n">
@@ -7147,6 +7621,9 @@
       <c r="N158" s="1" t="n">
         <v>210.7142857</v>
       </c>
+      <c r="O158" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="n">
@@ -7191,6 +7668,9 @@
       <c r="N159" s="1" t="n">
         <v>173.7089202</v>
       </c>
+      <c r="O159" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="n">
@@ -7235,6 +7715,9 @@
       <c r="N160" s="1" t="n">
         <v>189.5348837</v>
       </c>
+      <c r="O160" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="n">
@@ -7279,6 +7762,9 @@
       <c r="N161" s="1" t="n">
         <v>197.6744186</v>
       </c>
+      <c r="O161" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="n">
@@ -7323,6 +7809,9 @@
       <c r="N162" s="1" t="n">
         <v>151.4285714</v>
       </c>
+      <c r="O162" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="n">
@@ -7367,6 +7856,9 @@
       <c r="N163" s="1" t="n">
         <v>184.8591549</v>
       </c>
+      <c r="O163" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="n">
@@ -7411,6 +7903,9 @@
       <c r="N164" s="1" t="n">
         <v>178.8461538</v>
       </c>
+      <c r="O164" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="n">
@@ -7455,6 +7950,9 @@
       <c r="N165" s="1" t="n">
         <v>160</v>
       </c>
+      <c r="O165" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="n">
@@ -7499,6 +7997,9 @@
       <c r="N166" s="1" t="n">
         <v>161.6216216</v>
       </c>
+      <c r="O166" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="n">
@@ -7543,6 +8044,9 @@
       <c r="N167" s="1" t="n">
         <v>221.9387755</v>
       </c>
+      <c r="O167" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="n">
@@ -7587,6 +8091,9 @@
       <c r="N168" s="1" t="n">
         <v>235.0746269</v>
       </c>
+      <c r="O168" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="n">
@@ -7631,6 +8138,9 @@
       <c r="N169" s="1" t="n">
         <v>151.6587678</v>
       </c>
+      <c r="O169" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="n">
@@ -7675,6 +8185,9 @@
       <c r="N170" s="1" t="n">
         <v>227.2727273</v>
       </c>
+      <c r="O170" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="n">
@@ -7719,6 +8232,9 @@
       <c r="N171" s="1" t="n">
         <v>164.8241206</v>
       </c>
+      <c r="O171" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="172" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="n">
@@ -7763,6 +8279,9 @@
       <c r="N172" s="1" t="n">
         <v>182.4452555</v>
       </c>
+      <c r="O172" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="n">
@@ -7807,6 +8326,9 @@
       <c r="N173" s="1" t="n">
         <v>127.0053476</v>
       </c>
+      <c r="O173" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="n">
@@ -7851,6 +8373,9 @@
       <c r="N174" s="1" t="n">
         <v>190.6113537</v>
       </c>
+      <c r="O174" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="n">
@@ -7895,6 +8420,9 @@
       <c r="N175" s="1" t="n">
         <v>149.790795</v>
       </c>
+      <c r="O175" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="n">
@@ -7939,6 +8467,9 @@
       <c r="N176" s="1" t="n">
         <v>144.2307692</v>
       </c>
+      <c r="O176" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="n">
@@ -7983,6 +8514,9 @@
       <c r="N177" s="1" t="n">
         <v>147.7272727</v>
       </c>
+      <c r="O177" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="n">
@@ -8027,6 +8561,9 @@
       <c r="N178" s="1" t="n">
         <v>127.9411765</v>
       </c>
+      <c r="O178" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="n">
@@ -8071,6 +8608,9 @@
       <c r="N179" s="1" t="n">
         <v>235.4330709</v>
       </c>
+      <c r="O179" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="n">
@@ -8115,6 +8655,9 @@
       <c r="N180" s="1" t="n">
         <v>172.1991701</v>
       </c>
+      <c r="O180" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="n">
@@ -8159,6 +8702,9 @@
       <c r="N181" s="1" t="n">
         <v>150.9803922</v>
       </c>
+      <c r="O181" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="n">
@@ -8203,6 +8749,9 @@
       <c r="N182" s="1" t="n">
         <v>184.9285714</v>
       </c>
+      <c r="O182" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="n">
@@ -8247,6 +8796,9 @@
       <c r="N183" s="1" t="n">
         <v>237.259887</v>
       </c>
+      <c r="O183" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="n">
@@ -8291,6 +8843,9 @@
       <c r="N184" s="1" t="n">
         <v>243.5897436</v>
       </c>
+      <c r="O184" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="n">
@@ -8335,6 +8890,9 @@
       <c r="N185" s="1" t="n">
         <v>143.0188679</v>
       </c>
+      <c r="O185" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="n">
@@ -8379,6 +8937,9 @@
       <c r="N186" s="1" t="n">
         <v>163.9593909</v>
       </c>
+      <c r="O186" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="n">
@@ -8423,6 +8984,9 @@
       <c r="N187" s="1" t="n">
         <v>189.8734177</v>
       </c>
+      <c r="O187" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="188" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
@@ -8467,6 +9031,9 @@
       <c r="N188" s="1" t="n">
         <v>188.3248731</v>
       </c>
+      <c r="O188" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="n">
@@ -8511,6 +9078,9 @@
       <c r="N189" s="1" t="n">
         <v>168.6445783</v>
       </c>
+      <c r="O189" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="190" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="n">
@@ -8555,6 +9125,9 @@
       <c r="N190" s="1" t="n">
         <v>167.4418605</v>
       </c>
+      <c r="O190" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="n">
@@ -8599,6 +9172,9 @@
       <c r="N191" s="1" t="n">
         <v>182.5726141</v>
       </c>
+      <c r="O191" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="n">
@@ -8643,6 +9219,9 @@
       <c r="N192" s="1" t="n">
         <v>153.1914894</v>
       </c>
+      <c r="O192" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="n">
@@ -8687,6 +9266,9 @@
       <c r="N193" s="1" t="n">
         <v>172.6804124</v>
       </c>
+      <c r="O193" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="n">
@@ -8731,6 +9313,9 @@
       <c r="N194" s="1" t="n">
         <v>174.975</v>
       </c>
+      <c r="O194" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="195" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="n">
@@ -8775,6 +9360,9 @@
       <c r="N195" s="1" t="n">
         <v>158.5714286</v>
       </c>
+      <c r="O195" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="n">
@@ -8819,6 +9407,9 @@
       <c r="N196" s="1" t="n">
         <v>165.3543307</v>
       </c>
+      <c r="O196" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="197" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="n">
@@ -8863,6 +9454,9 @@
       <c r="N197" s="1" t="n">
         <v>191.1931818</v>
       </c>
+      <c r="O197" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="n">
@@ -8907,6 +9501,9 @@
       <c r="N198" s="1" t="n">
         <v>170.7836991</v>
       </c>
+      <c r="O198" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="199" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="n">
@@ -8951,6 +9548,9 @@
       <c r="N199" s="1" t="n">
         <v>199.4382022</v>
       </c>
+      <c r="O199" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="200" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="n">
@@ -8995,6 +9595,9 @@
       <c r="N200" s="1" t="n">
         <v>225</v>
       </c>
+      <c r="O200" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="201" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="n">
@@ -9039,6 +9642,9 @@
       <c r="N201" s="1" t="n">
         <v>175.8241758</v>
       </c>
+      <c r="O201" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="202" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="n">
@@ -9083,6 +9689,9 @@
       <c r="N202" s="1" t="n">
         <v>148.3870968</v>
       </c>
+      <c r="O202" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="203" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="n">
@@ -9127,6 +9736,9 @@
       <c r="N203" s="1" t="n">
         <v>210.4824561</v>
       </c>
+      <c r="O203" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="204" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="n">
@@ -9171,6 +9783,9 @@
       <c r="N204" s="1" t="n">
         <v>146.2555066</v>
       </c>
+      <c r="O204" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="205" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="n">
@@ -9215,6 +9830,9 @@
       <c r="N205" s="1" t="n">
         <v>145.7489879</v>
       </c>
+      <c r="O205" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="206" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="n">
@@ -9259,6 +9877,9 @@
       <c r="N206" s="1" t="n">
         <v>191.8867925</v>
       </c>
+      <c r="O206" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="n">
@@ -9303,6 +9924,9 @@
       <c r="N207" s="1" t="n">
         <v>126.8181818</v>
       </c>
+      <c r="O207" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="208" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="n">
@@ -9347,6 +9971,9 @@
       <c r="N208" s="1" t="n">
         <v>255</v>
       </c>
+      <c r="O208" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="209" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="n">
@@ -9391,6 +10018,9 @@
       <c r="N209" s="1" t="n">
         <v>148.005148</v>
       </c>
+      <c r="O209" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="210" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="n">
@@ -9435,6 +10065,9 @@
       <c r="N210" s="1" t="n">
         <v>137.0967742</v>
       </c>
+      <c r="O210" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="n">
@@ -9479,6 +10112,9 @@
       <c r="N211" s="1" t="n">
         <v>140.2439024</v>
       </c>
+      <c r="O211" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="212" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="n">
@@ -9523,6 +10159,9 @@
       <c r="N212" s="1" t="n">
         <v>252.3529412</v>
       </c>
+      <c r="O212" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="213" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="n">
@@ -9567,6 +10206,9 @@
       <c r="N213" s="1" t="n">
         <v>172.4137931</v>
       </c>
+      <c r="O213" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="214" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="n">
@@ -9611,6 +10253,9 @@
       <c r="N214" s="1" t="n">
         <v>146.9387755</v>
       </c>
+      <c r="O214" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="215" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="n">
@@ -9655,6 +10300,9 @@
       <c r="N215" s="1" t="n">
         <v>157.2614108</v>
       </c>
+      <c r="O215" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="216" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="n">
@@ -9699,6 +10347,9 @@
       <c r="N216" s="1" t="n">
         <v>161.9433198</v>
       </c>
+      <c r="O216" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="217" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="n">
@@ -9743,6 +10394,9 @@
       <c r="N217" s="1" t="n">
         <v>125</v>
       </c>
+      <c r="O217" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="218" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="n">
@@ -9787,6 +10441,9 @@
       <c r="N218" s="1" t="n">
         <v>189.6264368</v>
       </c>
+      <c r="O218" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="219" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="n">
@@ -9831,6 +10488,9 @@
       <c r="N219" s="1" t="n">
         <v>258.9694656</v>
       </c>
+      <c r="O219" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="220" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="n">
@@ -9875,6 +10535,9 @@
       <c r="N220" s="1" t="n">
         <v>155.5555556</v>
       </c>
+      <c r="O220" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="221" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="n">
@@ -9919,6 +10582,9 @@
       <c r="N221" s="1" t="n">
         <v>161.1570248</v>
       </c>
+      <c r="O221" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="222" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="n">
@@ -9963,6 +10629,9 @@
       <c r="N222" s="1" t="n">
         <v>186.7509728</v>
       </c>
+      <c r="O222" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="223" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="n">
@@ -10007,6 +10676,9 @@
       <c r="N223" s="1" t="n">
         <v>166.1016949</v>
       </c>
+      <c r="O223" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="224" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="n">
@@ -10051,6 +10723,9 @@
       <c r="N224" s="1" t="n">
         <v>154.2207792</v>
       </c>
+      <c r="O224" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="225" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="n">
@@ -10095,6 +10770,9 @@
       <c r="N225" s="1" t="n">
         <v>217.6470588</v>
       </c>
+      <c r="O225" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="226" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="n">
@@ -10139,6 +10817,9 @@
       <c r="N226" s="1" t="n">
         <v>200.5747126</v>
       </c>
+      <c r="O226" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="227" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="n">
@@ -10183,6 +10864,9 @@
       <c r="N227" s="1" t="n">
         <v>168.115942</v>
       </c>
+      <c r="O227" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="228" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="n">
@@ -10227,6 +10911,9 @@
       <c r="N228" s="1" t="n">
         <v>143.0232558</v>
       </c>
+      <c r="O228" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="229" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="n">
@@ -10271,6 +10958,9 @@
       <c r="N229" s="1" t="n">
         <v>151.489899</v>
       </c>
+      <c r="O229" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="230" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="n">
@@ -10315,6 +11005,9 @@
       <c r="N230" s="1" t="n">
         <v>142.8375</v>
       </c>
+      <c r="O230" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="231" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="n">
@@ -10359,6 +11052,9 @@
       <c r="N231" s="1" t="n">
         <v>174.7191011</v>
       </c>
+      <c r="O231" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="232" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="n">
@@ -10403,6 +11099,9 @@
       <c r="N232" s="1" t="n">
         <v>221.7741935</v>
       </c>
+      <c r="O232" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="233" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="n">
@@ -10447,6 +11146,9 @@
       <c r="N233" s="1" t="n">
         <v>186.6197183</v>
       </c>
+      <c r="O233" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="234" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="n">
@@ -10491,6 +11193,9 @@
       <c r="N234" s="1" t="n">
         <v>178.8957055</v>
       </c>
+      <c r="O234" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="235" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="n">
@@ -10535,6 +11240,9 @@
       <c r="N235" s="1" t="n">
         <v>163.197026</v>
       </c>
+      <c r="O235" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="236" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="n">
@@ -10579,6 +11287,9 @@
       <c r="N236" s="1" t="n">
         <v>170.5607477</v>
       </c>
+      <c r="O236" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="237" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="n">
@@ -10623,6 +11334,9 @@
       <c r="N237" s="1" t="n">
         <v>131.8897638</v>
       </c>
+      <c r="O237" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="238" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="n">
@@ -10667,6 +11381,9 @@
       <c r="N238" s="1" t="n">
         <v>189.4409938</v>
       </c>
+      <c r="O238" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="239" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="n">
@@ -10711,6 +11428,9 @@
       <c r="N239" s="1" t="n">
         <v>182.5842697</v>
       </c>
+      <c r="O239" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="240" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="n">
@@ -10755,6 +11475,9 @@
       <c r="N240" s="1" t="n">
         <v>155.9485531</v>
       </c>
+      <c r="O240" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="241" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="n">
@@ -10799,6 +11522,9 @@
       <c r="N241" s="1" t="n">
         <v>218.9655172</v>
       </c>
+      <c r="O241" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="242" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="n">
@@ -10843,6 +11569,9 @@
       <c r="N242" s="1" t="n">
         <v>123.2227488</v>
       </c>
+      <c r="O242" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="243" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="n">
@@ -10887,6 +11616,9 @@
       <c r="N243" s="1" t="n">
         <v>125</v>
       </c>
+      <c r="O243" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="244" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="n">
@@ -10931,6 +11663,9 @@
       <c r="N244" s="1" t="n">
         <v>143.5643564</v>
       </c>
+      <c r="O244" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="245" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="n">
@@ -10975,6 +11710,9 @@
       <c r="N245" s="1" t="n">
         <v>202.3255814</v>
       </c>
+      <c r="O245" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="246" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="n">
@@ -11019,6 +11757,9 @@
       <c r="N246" s="1" t="n">
         <v>212.962963</v>
       </c>
+      <c r="O246" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="247" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="n">
@@ -11063,6 +11804,9 @@
       <c r="N247" s="1" t="n">
         <v>166.9359223</v>
       </c>
+      <c r="O247" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="248" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="n">
@@ -11107,6 +11851,9 @@
       <c r="N248" s="1" t="n">
         <v>88.78504673</v>
       </c>
+      <c r="O248" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="249" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="n">
@@ -11151,6 +11898,9 @@
       <c r="N249" s="1" t="n">
         <v>186.8556701</v>
       </c>
+      <c r="O249" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="250" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="n">
@@ -11195,6 +11945,9 @@
       <c r="N250" s="1" t="n">
         <v>174.8427673</v>
       </c>
+      <c r="O250" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="251" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="n">
@@ -11239,6 +11992,9 @@
       <c r="N251" s="1" t="n">
         <v>139.9253731</v>
       </c>
+      <c r="O251" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="252" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="n">
@@ -11283,6 +12039,9 @@
       <c r="N252" s="1" t="n">
         <v>207.1895425</v>
       </c>
+      <c r="O252" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="253" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="n">
@@ -11327,6 +12086,9 @@
       <c r="N253" s="1" t="n">
         <v>206.25</v>
       </c>
+      <c r="O253" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="254" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="n">
@@ -11371,6 +12133,9 @@
       <c r="N254" s="1" t="n">
         <v>121.5384615</v>
       </c>
+      <c r="O254" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="255" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="n">
@@ -11415,6 +12180,9 @@
       <c r="N255" s="1" t="n">
         <v>175.5725191</v>
       </c>
+      <c r="O255" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="256" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="n">
@@ -11459,6 +12227,9 @@
       <c r="N256" s="1" t="n">
         <v>214.2857143</v>
       </c>
+      <c r="O256" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="257" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="n">
@@ -11503,6 +12274,9 @@
       <c r="N257" s="1" t="n">
         <v>202.8301887</v>
       </c>
+      <c r="O257" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="258" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="n">
@@ -11547,6 +12321,9 @@
       <c r="N258" s="1" t="n">
         <v>210</v>
       </c>
+      <c r="O258" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="259" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="n">
@@ -11591,6 +12368,9 @@
       <c r="N259" s="1" t="n">
         <v>247.9338843</v>
       </c>
+      <c r="O259" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="260" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="n">
@@ -11635,6 +12415,9 @@
       <c r="N260" s="1" t="n">
         <v>177.4647887</v>
       </c>
+      <c r="O260" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="261" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="n">
@@ -11679,6 +12462,9 @@
       <c r="N261" s="1" t="n">
         <v>163.0851064</v>
       </c>
+      <c r="O261" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="262" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="n">
@@ -11723,6 +12509,9 @@
       <c r="N262" s="1" t="n">
         <v>149.4252874</v>
       </c>
+      <c r="O262" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="263" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="n">
@@ -11767,6 +12556,9 @@
       <c r="N263" s="1" t="n">
         <v>180</v>
       </c>
+      <c r="O263" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="264" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="n">
@@ -11811,6 +12603,9 @@
       <c r="N264" s="1" t="n">
         <v>122.1543408</v>
       </c>
+      <c r="O264" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="265" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="n">
@@ -11855,6 +12650,9 @@
       <c r="N265" s="1" t="n">
         <v>287.5</v>
       </c>
+      <c r="O265" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="266" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="n">
@@ -11899,6 +12697,9 @@
       <c r="N266" s="1" t="n">
         <v>121.4733542</v>
       </c>
+      <c r="O266" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="267" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="n">
@@ -11943,6 +12744,9 @@
       <c r="N267" s="1" t="n">
         <v>135.6932153</v>
       </c>
+      <c r="O267" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="268" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="n">
@@ -11987,6 +12791,9 @@
       <c r="N268" s="1" t="n">
         <v>149.6212121</v>
       </c>
+      <c r="O268" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="269" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="n">
@@ -12031,6 +12838,9 @@
       <c r="N269" s="1" t="n">
         <v>130.7189542</v>
       </c>
+      <c r="O269" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="270" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="n">
@@ -12075,6 +12885,9 @@
       <c r="N270" s="1" t="n">
         <v>149.7409326</v>
       </c>
+      <c r="O270" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="271" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="n">
@@ -12119,6 +12932,9 @@
       <c r="N271" s="1" t="n">
         <v>237.6229508</v>
       </c>
+      <c r="O271" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="272" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="n">
@@ -12163,6 +12979,9 @@
       <c r="N272" s="1" t="n">
         <v>149.7767857</v>
       </c>
+      <c r="O272" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="273" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="n">
@@ -12207,6 +13026,9 @@
       <c r="N273" s="1" t="n">
         <v>151.1693548</v>
       </c>
+      <c r="O273" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="274" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="n">
@@ -12251,6 +13073,9 @@
       <c r="N274" s="1" t="n">
         <v>221.9512195</v>
       </c>
+      <c r="O274" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="275" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="n">
@@ -12295,6 +13120,9 @@
       <c r="N275" s="1" t="n">
         <v>138.5064935</v>
       </c>
+      <c r="O275" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="276" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="n">
@@ -12339,6 +13167,9 @@
       <c r="N276" s="1" t="n">
         <v>158.4158416</v>
       </c>
+      <c r="O276" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="277" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="n">
@@ -12383,6 +13214,9 @@
       <c r="N277" s="1" t="n">
         <v>172.4137931</v>
       </c>
+      <c r="O277" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="278" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="n">
@@ -12427,6 +13261,9 @@
       <c r="N278" s="1" t="n">
         <v>192.3076923</v>
       </c>
+      <c r="O278" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="279" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="n">
@@ -12471,6 +13308,9 @@
       <c r="N279" s="1" t="n">
         <v>143.0517711</v>
       </c>
+      <c r="O279" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="280" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="n">
@@ -12515,6 +13355,9 @@
       <c r="N280" s="1" t="n">
         <v>159.5744681</v>
       </c>
+      <c r="O280" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="281" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="n">
@@ -12559,6 +13402,9 @@
       <c r="N281" s="1" t="n">
         <v>240.5660377</v>
       </c>
+      <c r="O281" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="282" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="n">
@@ -12603,6 +13449,9 @@
       <c r="N282" s="1" t="n">
         <v>108.5858586</v>
       </c>
+      <c r="O282" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="283" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="n">
@@ -12647,6 +13496,9 @@
       <c r="N283" s="1" t="n">
         <v>202.81</v>
       </c>
+      <c r="O283" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="284" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="n">
@@ -12691,6 +13543,9 @@
       <c r="N284" s="1" t="n">
         <v>158.9958159</v>
       </c>
+      <c r="O284" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="285" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="n">
@@ -12735,6 +13590,9 @@
       <c r="N285" s="1" t="n">
         <v>184.4652406</v>
       </c>
+      <c r="O285" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="286" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="n">
@@ -12779,6 +13637,9 @@
       <c r="N286" s="1" t="n">
         <v>131.0483871</v>
       </c>
+      <c r="O286" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="287" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="n">
@@ -12823,6 +13684,9 @@
       <c r="N287" s="1" t="n">
         <v>186.4253394</v>
       </c>
+      <c r="O287" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="288" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="n">
@@ -12867,6 +13731,9 @@
       <c r="N288" s="1" t="n">
         <v>141.4634146</v>
       </c>
+      <c r="O288" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="289" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="n">
@@ -12911,6 +13778,9 @@
       <c r="N289" s="1" t="n">
         <v>128.9255014</v>
       </c>
+      <c r="O289" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="290" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="n">
@@ -12955,6 +13825,9 @@
       <c r="N290" s="1" t="n">
         <v>139.5348837</v>
       </c>
+      <c r="O290" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="291" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="n">
@@ -12999,6 +13872,9 @@
       <c r="N291" s="1" t="n">
         <v>211.9205298</v>
       </c>
+      <c r="O291" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="292" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="n">
@@ -13043,6 +13919,9 @@
       <c r="N292" s="1" t="n">
         <v>429.3676471</v>
       </c>
+      <c r="O292" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="293" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="n">
@@ -13087,6 +13966,9 @@
       <c r="N293" s="1" t="n">
         <v>167.5531915</v>
       </c>
+      <c r="O293" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="294" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="n">
@@ -13131,6 +14013,9 @@
       <c r="N294" s="1" t="n">
         <v>125.9398496</v>
       </c>
+      <c r="O294" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="295" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="n">
@@ -13175,6 +14060,9 @@
       <c r="N295" s="1" t="n">
         <v>174.6820809</v>
       </c>
+      <c r="O295" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="296" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="n">
@@ -13219,6 +14107,9 @@
       <c r="N296" s="1" t="n">
         <v>225.873494</v>
       </c>
+      <c r="O296" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="297" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="n">
@@ -13263,6 +14154,9 @@
       <c r="N297" s="1" t="n">
         <v>177.0949721</v>
       </c>
+      <c r="O297" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="298" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="n">
@@ -13307,6 +14201,9 @@
       <c r="N298" s="1" t="n">
         <v>257.9787234</v>
       </c>
+      <c r="O298" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="299" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="n">
@@ -13351,6 +14248,9 @@
       <c r="N299" s="1" t="n">
         <v>135.8024691</v>
       </c>
+      <c r="O299" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="300" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="n">
@@ -13395,6 +14295,9 @@
       <c r="N300" s="1" t="n">
         <v>205.6451613</v>
       </c>
+      <c r="O300" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="301" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="n">
@@ -13439,6 +14342,9 @@
       <c r="N301" s="1" t="n">
         <v>159.3886463</v>
       </c>
+      <c r="O301" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="302" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="n">
@@ -13483,6 +14389,9 @@
       <c r="N302" s="1" t="n">
         <v>158.4115523</v>
       </c>
+      <c r="O302" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="303" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="n">
@@ -13527,6 +14436,9 @@
       <c r="N303" s="1" t="n">
         <v>139.5348837</v>
       </c>
+      <c r="O303" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="304" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="n">
@@ -13571,6 +14483,9 @@
       <c r="N304" s="1" t="n">
         <v>178.8732394</v>
       </c>
+      <c r="O304" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="305" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="n">
@@ -13615,6 +14530,9 @@
       <c r="N305" s="1" t="n">
         <v>197.265625</v>
       </c>
+      <c r="O305" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="306" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="n">
@@ -13659,6 +14577,9 @@
       <c r="N306" s="1" t="n">
         <v>204.3010753</v>
       </c>
+      <c r="O306" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="307" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="n">
@@ -13703,6 +14624,9 @@
       <c r="N307" s="1" t="n">
         <v>161.3333333</v>
       </c>
+      <c r="O307" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="308" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="n">
@@ -13747,6 +14671,9 @@
       <c r="N308" s="1" t="n">
         <v>140.5405405</v>
       </c>
+      <c r="O308" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="309" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="n">
@@ -13791,6 +14718,9 @@
       <c r="N309" s="1" t="n">
         <v>158.1069959</v>
       </c>
+      <c r="O309" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="310" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="n">
@@ -13835,6 +14765,9 @@
       <c r="N310" s="1" t="n">
         <v>225.4901961</v>
       </c>
+      <c r="O310" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="311" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="n">
@@ -13879,6 +14812,9 @@
       <c r="N311" s="1" t="n">
         <v>194.53125</v>
       </c>
+      <c r="O311" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="312" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="n">
@@ -13923,6 +14859,9 @@
       <c r="N312" s="1" t="n">
         <v>197.3829201</v>
       </c>
+      <c r="O312" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="313" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="n">
@@ -13967,6 +14906,9 @@
       <c r="N313" s="1" t="n">
         <v>157.8947368</v>
       </c>
+      <c r="O313" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="314" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="n">
@@ -14011,6 +14953,9 @@
       <c r="N314" s="1" t="n">
         <v>205.8823529</v>
       </c>
+      <c r="O314" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="315" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="n">
@@ -14055,6 +15000,9 @@
       <c r="N315" s="1" t="n">
         <v>172.6438849</v>
       </c>
+      <c r="O315" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="316" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="n">
@@ -14099,6 +15047,9 @@
       <c r="N316" s="1" t="n">
         <v>205.8823529</v>
       </c>
+      <c r="O316" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="317" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="n">
@@ -14143,6 +15094,9 @@
       <c r="N317" s="1" t="n">
         <v>143.3349259</v>
       </c>
+      <c r="O317" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="318" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="n">
@@ -14187,6 +15141,9 @@
       <c r="N318" s="1" t="n">
         <v>142.5438596</v>
       </c>
+      <c r="O318" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="319" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="n">
@@ -14231,6 +15188,9 @@
       <c r="N319" s="1" t="n">
         <v>276.3888889</v>
       </c>
+      <c r="O319" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="320" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="n">
@@ -14275,6 +15235,9 @@
       <c r="N320" s="1" t="n">
         <v>147.9591837</v>
       </c>
+      <c r="O320" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="321" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="n">
@@ -14319,6 +15282,9 @@
       <c r="N321" s="1" t="n">
         <v>286.0068259</v>
       </c>
+      <c r="O321" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="322" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="n">
@@ -14363,6 +15329,9 @@
       <c r="N322" s="1" t="n">
         <v>110.0558659</v>
       </c>
+      <c r="O322" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="323" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="n">
@@ -14407,6 +15376,9 @@
       <c r="N323" s="1" t="n">
         <v>208.5582822</v>
       </c>
+      <c r="O323" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="324" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="n">
@@ -14451,6 +15423,9 @@
       <c r="N324" s="1" t="n">
         <v>171.0144928</v>
       </c>
+      <c r="O324" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="325" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="n">
@@ -14495,6 +15470,9 @@
       <c r="N325" s="1" t="n">
         <v>136.0544218</v>
       </c>
+      <c r="O325" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="326" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="n">
@@ -14539,6 +15517,9 @@
       <c r="N326" s="1" t="n">
         <v>245.8333333</v>
       </c>
+      <c r="O326" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="327" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="n">
@@ -14583,6 +15564,9 @@
       <c r="N327" s="1" t="n">
         <v>169.9382716</v>
       </c>
+      <c r="O327" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="328" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="n">
@@ -14627,6 +15611,9 @@
       <c r="N328" s="1" t="n">
         <v>146.3414634</v>
       </c>
+      <c r="O328" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="329" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="n">
@@ -14671,6 +15658,9 @@
       <c r="N329" s="1" t="n">
         <v>213.1782946</v>
       </c>
+      <c r="O329" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="330" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="n">
@@ -14715,6 +15705,9 @@
       <c r="N330" s="1" t="n">
         <v>260.9022556</v>
       </c>
+      <c r="O330" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="331" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="n">
@@ -14759,6 +15752,9 @@
       <c r="N331" s="1" t="n">
         <v>227.6422764</v>
       </c>
+      <c r="O331" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="332" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="n">
@@ -14803,6 +15799,9 @@
       <c r="N332" s="1" t="n">
         <v>164.7619048</v>
       </c>
+      <c r="O332" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="333" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="n">
@@ -14847,6 +15846,9 @@
       <c r="N333" s="1" t="n">
         <v>176.744186</v>
       </c>
+      <c r="O333" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="334" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="n">
@@ -14891,6 +15893,9 @@
       <c r="N334" s="1" t="n">
         <v>170.1030928</v>
       </c>
+      <c r="O334" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="335" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="n">
@@ -14935,6 +15940,9 @@
       <c r="N335" s="1" t="n">
         <v>163.3663366</v>
       </c>
+      <c r="O335" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="336" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="n">
@@ -14979,6 +15987,9 @@
       <c r="N336" s="1" t="n">
         <v>252.4752475</v>
       </c>
+      <c r="O336" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="337" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="n">
@@ -15023,6 +16034,9 @@
       <c r="N337" s="1" t="n">
         <v>177.1276596</v>
       </c>
+      <c r="O337" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="338" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="1" t="n">
@@ -15067,6 +16081,9 @@
       <c r="N338" s="1" t="n">
         <v>191.4285714</v>
       </c>
+      <c r="O338" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="339" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="n">
@@ -15111,6 +16128,9 @@
       <c r="N339" s="1" t="n">
         <v>144.6428571</v>
       </c>
+      <c r="O339" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="340" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="n">
@@ -15155,6 +16175,9 @@
       <c r="N340" s="1" t="n">
         <v>187.1287129</v>
       </c>
+      <c r="O340" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="341" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="n">
@@ -15199,6 +16222,9 @@
       <c r="N341" s="1" t="n">
         <v>180.6629834</v>
       </c>
+      <c r="O341" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="342" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="n">
@@ -15243,6 +16269,9 @@
       <c r="N342" s="1" t="n">
         <v>155.7620818</v>
       </c>
+      <c r="O342" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="343" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="n">
@@ -15287,6 +16316,9 @@
       <c r="N343" s="1" t="n">
         <v>150.7692308</v>
       </c>
+      <c r="O343" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="344" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A344" s="1" t="n">
@@ -15331,6 +16363,9 @@
       <c r="N344" s="1" t="n">
         <v>195.8762887</v>
       </c>
+      <c r="O344" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="345" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A345" s="1" t="n">
@@ -15375,6 +16410,9 @@
       <c r="N345" s="1" t="n">
         <v>127.6223776</v>
       </c>
+      <c r="O345" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="346" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A346" s="1" t="n">
@@ -15419,6 +16457,9 @@
       <c r="N346" s="1" t="n">
         <v>193.7799043</v>
       </c>
+      <c r="O346" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="347" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A347" s="1" t="n">
@@ -15463,6 +16504,9 @@
       <c r="N347" s="1" t="n">
         <v>172.6457399</v>
       </c>
+      <c r="O347" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="348" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A348" s="1" t="n">
@@ -15507,6 +16551,9 @@
       <c r="N348" s="1" t="n">
         <v>165.3587444</v>
       </c>
+      <c r="O348" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="349" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A349" s="1" t="n">
@@ -15551,6 +16598,9 @@
       <c r="N349" s="1" t="n">
         <v>178.8135593</v>
       </c>
+      <c r="O349" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="350" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A350" s="1" t="n">
@@ -15595,6 +16645,9 @@
       <c r="N350" s="1" t="n">
         <v>256.4102564</v>
       </c>
+      <c r="O350" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="351" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A351" s="1" t="n">
@@ -15639,6 +16692,9 @@
       <c r="N351" s="1" t="n">
         <v>125</v>
       </c>
+      <c r="O351" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="352" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A352" s="1" t="n">
@@ -15683,6 +16739,9 @@
       <c r="N352" s="1" t="n">
         <v>185.483871</v>
       </c>
+      <c r="O352" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="353" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A353" s="1" t="n">
@@ -15727,6 +16786,9 @@
       <c r="N353" s="1" t="n">
         <v>148.7068966</v>
       </c>
+      <c r="O353" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="354" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A354" s="1" t="n">
@@ -15771,6 +16833,9 @@
       <c r="N354" s="1" t="n">
         <v>143.9688716</v>
       </c>
+      <c r="O354" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="355" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A355" s="1" t="n">
@@ -15815,6 +16880,9 @@
       <c r="N355" s="1" t="n">
         <v>229.5069444</v>
       </c>
+      <c r="O355" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="356" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A356" s="1" t="n">
@@ -15859,6 +16927,9 @@
       <c r="N356" s="1" t="n">
         <v>138.7596899</v>
       </c>
+      <c r="O356" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="357" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A357" s="1" t="n">
@@ -15903,6 +16974,9 @@
       <c r="N357" s="1" t="n">
         <v>136.6906475</v>
       </c>
+      <c r="O357" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="358" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A358" s="1" t="n">
@@ -15947,6 +17021,9 @@
       <c r="N358" s="1" t="n">
         <v>135.1694915</v>
       </c>
+      <c r="O358" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="359" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A359" s="1" t="n">
@@ -15991,6 +17068,9 @@
       <c r="N359" s="1" t="n">
         <v>207.2992701</v>
       </c>
+      <c r="O359" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="360" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A360" s="1" t="n">
@@ -16035,6 +17115,9 @@
       <c r="N360" s="1" t="n">
         <v>187.8453039</v>
       </c>
+      <c r="O360" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="361" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A361" s="1" t="n">
@@ -16079,6 +17162,9 @@
       <c r="N361" s="1" t="n">
         <v>175.5555556</v>
       </c>
+      <c r="O361" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="362" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A362" s="1" t="n">
@@ -16123,6 +17209,9 @@
       <c r="N362" s="1" t="n">
         <v>164.516129</v>
       </c>
+      <c r="O362" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="363" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A363" s="1" t="n">
@@ -16167,6 +17256,9 @@
       <c r="N363" s="1" t="n">
         <v>180.3468208</v>
       </c>
+      <c r="O363" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="364" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A364" s="1" t="n">
@@ -16211,6 +17303,9 @@
       <c r="N364" s="1" t="n">
         <v>244.9541284</v>
       </c>
+      <c r="O364" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="365" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A365" s="1" t="n">
@@ -16255,6 +17350,9 @@
       <c r="N365" s="1" t="n">
         <v>184</v>
       </c>
+      <c r="O365" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="366" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A366" s="1" t="n">
@@ -16299,6 +17397,9 @@
       <c r="N366" s="1" t="n">
         <v>195.9183673</v>
       </c>
+      <c r="O366" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="367" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A367" s="1" t="n">
@@ -16343,6 +17444,9 @@
       <c r="N367" s="1" t="n">
         <v>156.1403509</v>
       </c>
+      <c r="O367" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="368" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A368" s="1" t="n">
@@ -16387,6 +17491,9 @@
       <c r="N368" s="1" t="n">
         <v>186.0465116</v>
       </c>
+      <c r="O368" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="369" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A369" s="1" t="n">
@@ -16431,6 +17538,9 @@
       <c r="N369" s="1" t="n">
         <v>192.1348315</v>
       </c>
+      <c r="O369" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="370" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A370" s="1" t="n">
@@ -16475,6 +17585,9 @@
       <c r="N370" s="1" t="n">
         <v>158.6538462</v>
       </c>
+      <c r="O370" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="371" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A371" s="1" t="n">
@@ -16519,6 +17632,9 @@
       <c r="N371" s="1" t="n">
         <v>152.7777778</v>
       </c>
+      <c r="O371" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="372" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A372" s="1" t="n">
@@ -16563,6 +17679,9 @@
       <c r="N372" s="1" t="n">
         <v>156.7099567</v>
       </c>
+      <c r="O372" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="373" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A373" s="1" t="n">
@@ -16607,6 +17726,9 @@
       <c r="N373" s="1" t="n">
         <v>173.7804878</v>
       </c>
+      <c r="O373" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="374" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A374" s="1" t="n">
@@ -16651,6 +17773,9 @@
       <c r="N374" s="1" t="n">
         <v>169.2708333</v>
       </c>
+      <c r="O374" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="375" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A375" s="1" t="n">
@@ -16695,6 +17820,9 @@
       <c r="N375" s="1" t="n">
         <v>209.2511013</v>
       </c>
+      <c r="O375" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="376" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A376" s="1" t="n">
@@ -16739,6 +17867,9 @@
       <c r="N376" s="1" t="n">
         <v>139.5027624</v>
       </c>
+      <c r="O376" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="377" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A377" s="1" t="n">
@@ -16783,6 +17914,9 @@
       <c r="N377" s="1" t="n">
         <v>329.95</v>
       </c>
+      <c r="O377" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="378" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A378" s="1" t="n">
@@ -16827,6 +17961,9 @@
       <c r="N378" s="1" t="n">
         <v>181.1594203</v>
       </c>
+      <c r="O378" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="379" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A379" s="1" t="n">
@@ -16871,6 +18008,9 @@
       <c r="N379" s="1" t="n">
         <v>176.5027322</v>
       </c>
+      <c r="O379" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="380" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A380" s="1" t="n">
@@ -16915,6 +18055,9 @@
       <c r="N380" s="1" t="n">
         <v>191.1764706</v>
       </c>
+      <c r="O380" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="381" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A381" s="1" t="n">
@@ -16959,6 +18102,9 @@
       <c r="N381" s="1" t="n">
         <v>271.7770035</v>
       </c>
+      <c r="O381" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="382" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A382" s="1" t="n">
@@ -17003,6 +18149,9 @@
       <c r="N382" s="1" t="n">
         <v>135.9605911</v>
       </c>
+      <c r="O382" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="383" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A383" s="1" t="n">
@@ -17047,6 +18196,9 @@
       <c r="N383" s="1" t="n">
         <v>211.440678</v>
       </c>
+      <c r="O383" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="384" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A384" s="1" t="n">
@@ -17091,6 +18243,9 @@
       <c r="N384" s="1" t="n">
         <v>218.4466019</v>
       </c>
+      <c r="O384" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="385" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A385" s="1" t="n">
@@ -17135,6 +18290,9 @@
       <c r="N385" s="1" t="n">
         <v>156.5764925</v>
       </c>
+      <c r="O385" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="386" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A386" s="1" t="n">
@@ -17179,6 +18337,9 @@
       <c r="N386" s="1" t="n">
         <v>245.0549451</v>
       </c>
+      <c r="O386" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="387" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A387" s="1" t="n">
@@ -17223,6 +18384,9 @@
       <c r="N387" s="1" t="n">
         <v>113.5531136</v>
       </c>
+      <c r="O387" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="388" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A388" s="1" t="n">
@@ -17267,6 +18431,9 @@
       <c r="N388" s="1" t="n">
         <v>211.0169492</v>
       </c>
+      <c r="O388" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="389" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A389" s="1" t="n">
@@ -17311,6 +18478,9 @@
       <c r="N389" s="1" t="n">
         <v>130.8673469</v>
       </c>
+      <c r="O389" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="390" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A390" s="1" t="n">
@@ -17355,6 +18525,9 @@
       <c r="N390" s="1" t="n">
         <v>247.2527473</v>
       </c>
+      <c r="O390" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="391" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A391" s="1" t="n">
@@ -17399,6 +18572,9 @@
       <c r="N391" s="1" t="n">
         <v>171.2328767</v>
       </c>
+      <c r="O391" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="392" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A392" s="1" t="n">
@@ -17443,6 +18619,9 @@
       <c r="N392" s="1" t="n">
         <v>145.2380952</v>
       </c>
+      <c r="O392" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="393" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A393" s="1" t="n">
@@ -17487,6 +18666,9 @@
       <c r="N393" s="1" t="n">
         <v>180.952381</v>
       </c>
+      <c r="O393" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="394" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A394" s="1" t="n">
@@ -17531,6 +18713,9 @@
       <c r="N394" s="1" t="n">
         <v>175</v>
       </c>
+      <c r="O394" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="395" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A395" s="1" t="n">
@@ -17575,6 +18760,9 @@
       <c r="N395" s="1" t="n">
         <v>167.896679</v>
       </c>
+      <c r="O395" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="396" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A396" s="1" t="n">
@@ -17619,6 +18807,9 @@
       <c r="N396" s="1" t="n">
         <v>137.366548</v>
       </c>
+      <c r="O396" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="397" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A397" s="1" t="n">
@@ -17663,6 +18854,9 @@
       <c r="N397" s="1" t="n">
         <v>182.0754717</v>
       </c>
+      <c r="O397" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="398" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A398" s="1" t="n">
@@ -17707,6 +18901,9 @@
       <c r="N398" s="1" t="n">
         <v>209.6219931</v>
       </c>
+      <c r="O398" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="399" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A399" s="1" t="n">
@@ -17751,6 +18948,9 @@
       <c r="N399" s="1" t="n">
         <v>115.2173913</v>
       </c>
+      <c r="O399" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="400" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A400" s="1" t="n">
@@ -17795,6 +18995,9 @@
       <c r="N400" s="1" t="n">
         <v>189.3333333</v>
       </c>
+      <c r="O400" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="401" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="n">
@@ -17839,6 +19042,9 @@
       <c r="N401" s="1" t="n">
         <v>197.740113</v>
       </c>
+      <c r="O401" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="402" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A402" s="1" t="n">
@@ -17883,6 +19089,9 @@
       <c r="N402" s="1" t="n">
         <v>170.1030928</v>
       </c>
+      <c r="O402" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="403" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A403" s="1" t="n">
@@ -17927,6 +19136,9 @@
       <c r="N403" s="1" t="n">
         <v>128.8209607</v>
       </c>
+      <c r="O403" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="404" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A404" s="1" t="n">
@@ -17971,6 +19183,9 @@
       <c r="N404" s="1" t="n">
         <v>240.2822581</v>
       </c>
+      <c r="O404" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="405" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A405" s="1" t="n">
@@ -18015,6 +19230,9 @@
       <c r="N405" s="1" t="n">
         <v>178.8617886</v>
       </c>
+      <c r="O405" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="406" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A406" s="1" t="n">
@@ -18059,6 +19277,9 @@
       <c r="N406" s="1" t="n">
         <v>119.9563953</v>
       </c>
+      <c r="O406" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="407" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A407" s="1" t="n">
@@ -18103,6 +19324,9 @@
       <c r="N407" s="1" t="n">
         <v>197.0930233</v>
       </c>
+      <c r="O407" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="408" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A408" s="1" t="n">
@@ -18147,6 +19371,9 @@
       <c r="N408" s="1" t="n">
         <v>143.4108527</v>
       </c>
+      <c r="O408" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="409" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A409" s="1" t="n">
@@ -18191,6 +19418,9 @@
       <c r="N409" s="1" t="n">
         <v>176.3043478</v>
       </c>
+      <c r="O409" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="410" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A410" s="1" t="n">
@@ -18235,6 +19465,9 @@
       <c r="N410" s="1" t="n">
         <v>174.3801653</v>
       </c>
+      <c r="O410" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="411" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A411" s="1" t="n">
@@ -18279,6 +19512,9 @@
       <c r="N411" s="1" t="n">
         <v>198.3843537</v>
       </c>
+      <c r="O411" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="412" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A412" s="1" t="n">
@@ -18323,6 +19559,9 @@
       <c r="N412" s="1" t="n">
         <v>159.4982079</v>
       </c>
+      <c r="O412" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="413" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A413" s="1" t="n">
@@ -18367,6 +19606,9 @@
       <c r="N413" s="1" t="n">
         <v>153.3333333</v>
       </c>
+      <c r="O413" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="414" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A414" s="1" t="n">
@@ -18411,6 +19653,9 @@
       <c r="N414" s="1" t="n">
         <v>201.0309278</v>
       </c>
+      <c r="O414" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="415" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A415" s="1" t="n">
@@ -18455,6 +19700,9 @@
       <c r="N415" s="1" t="n">
         <v>192.139738</v>
       </c>
+      <c r="O415" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="416" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A416" s="1" t="n">
@@ -18499,6 +19747,9 @@
       <c r="N416" s="1" t="n">
         <v>194.0104167</v>
       </c>
+      <c r="O416" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="417" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A417" s="1" t="n">
@@ -18543,6 +19794,9 @@
       <c r="N417" s="1" t="n">
         <v>180.7894737</v>
       </c>
+      <c r="O417" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="418" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A418" s="1" t="n">
@@ -18587,6 +19841,9 @@
       <c r="N418" s="1" t="n">
         <v>182.2147651</v>
       </c>
+      <c r="O418" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="419" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A419" s="1" t="n">
@@ -18631,6 +19888,9 @@
       <c r="N419" s="1" t="n">
         <v>103.6866359</v>
       </c>
+      <c r="O419" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="420" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A420" s="1" t="n">
@@ -18675,6 +19935,9 @@
       <c r="N420" s="1" t="n">
         <v>157.1571906</v>
       </c>
+      <c r="O420" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="421" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A421" s="1" t="n">
@@ -18719,6 +19982,9 @@
       <c r="N421" s="1" t="n">
         <v>152.7777778</v>
       </c>
+      <c r="O421" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="422" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A422" s="1" t="n">
@@ -18763,6 +20029,9 @@
       <c r="N422" s="1" t="n">
         <v>184.4919786</v>
       </c>
+      <c r="O422" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="423" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A423" s="1" t="n">
@@ -18807,6 +20076,9 @@
       <c r="N423" s="1" t="n">
         <v>170.6333333</v>
       </c>
+      <c r="O423" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="424" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A424" s="1" t="n">
@@ -18851,6 +20123,9 @@
       <c r="N424" s="1" t="n">
         <v>225</v>
       </c>
+      <c r="O424" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="425" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A425" s="1" t="n">
@@ -18895,6 +20170,9 @@
       <c r="N425" s="1" t="n">
         <v>229.6</v>
       </c>
+      <c r="O425" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="426" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A426" s="1" t="n">
@@ -18939,6 +20217,9 @@
       <c r="N426" s="1" t="n">
         <v>207.0063694</v>
       </c>
+      <c r="O426" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="427" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A427" s="1" t="n">
@@ -18983,6 +20264,9 @@
       <c r="N427" s="1" t="n">
         <v>155.0887978</v>
       </c>
+      <c r="O427" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="428" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A428" s="1" t="n">
@@ -19027,6 +20311,9 @@
       <c r="N428" s="1" t="n">
         <v>125</v>
       </c>
+      <c r="O428" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="429" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A429" s="1" t="n">
@@ -19071,6 +20358,9 @@
       <c r="N429" s="1" t="n">
         <v>207.5471698</v>
       </c>
+      <c r="O429" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="430" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A430" s="1" t="n">
@@ -19115,6 +20405,9 @@
       <c r="N430" s="1" t="n">
         <v>159.0163934</v>
       </c>
+      <c r="O430" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="431" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A431" s="1" t="n">
@@ -19159,6 +20452,9 @@
       <c r="N431" s="1" t="n">
         <v>182.1428571</v>
       </c>
+      <c r="O431" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="432" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A432" s="1" t="n">
@@ -19203,6 +20499,9 @@
       <c r="N432" s="1" t="n">
         <v>178.5714286</v>
       </c>
+      <c r="O432" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="433" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A433" s="1" t="n">
@@ -19247,6 +20546,9 @@
       <c r="N433" s="1" t="n">
         <v>166.1616162</v>
       </c>
+      <c r="O433" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="434" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A434" s="1" t="n">
@@ -19291,6 +20593,9 @@
       <c r="N434" s="1" t="n">
         <v>194.7204969</v>
       </c>
+      <c r="O434" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="435" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A435" s="1" t="n">
@@ -19335,6 +20640,9 @@
       <c r="N435" s="1" t="n">
         <v>164.4444444</v>
       </c>
+      <c r="O435" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="436" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A436" s="1" t="n">
@@ -19379,6 +20687,9 @@
       <c r="N436" s="1" t="n">
         <v>134.6846847</v>
       </c>
+      <c r="O436" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="437" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A437" s="1" t="n">
@@ -19423,6 +20734,9 @@
       <c r="N437" s="1" t="n">
         <v>155.3964758</v>
       </c>
+      <c r="O437" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="438" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A438" s="1" t="n">
@@ -19467,6 +20781,9 @@
       <c r="N438" s="1" t="n">
         <v>227.2058824</v>
       </c>
+      <c r="O438" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="439" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A439" s="1" t="n">
@@ -19511,6 +20828,9 @@
       <c r="N439" s="1" t="n">
         <v>243.4782609</v>
       </c>
+      <c r="O439" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="440" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A440" s="1" t="n">
@@ -19555,6 +20875,9 @@
       <c r="N440" s="1" t="n">
         <v>147.5</v>
       </c>
+      <c r="O440" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="441" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A441" s="1" t="n">
@@ -19599,6 +20922,9 @@
       <c r="N441" s="1" t="n">
         <v>193.2624113</v>
       </c>
+      <c r="O441" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="442" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A442" s="1" t="n">
@@ -19643,6 +20969,9 @@
       <c r="N442" s="1" t="n">
         <v>215.0537634</v>
       </c>
+      <c r="O442" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="443" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A443" s="1" t="n">
@@ -19687,6 +21016,9 @@
       <c r="N443" s="1" t="n">
         <v>177.5986842</v>
       </c>
+      <c r="O443" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="444" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A444" s="1" t="n">
@@ -19731,6 +21063,9 @@
       <c r="N444" s="1" t="n">
         <v>151.3243243</v>
       </c>
+      <c r="O444" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="445" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A445" s="1" t="n">
@@ -19775,6 +21110,9 @@
       <c r="N445" s="1" t="n">
         <v>193.0379747</v>
       </c>
+      <c r="O445" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="446" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A446" s="1" t="n">
@@ -19819,6 +21157,9 @@
       <c r="N446" s="1" t="n">
         <v>168.7165775</v>
       </c>
+      <c r="O446" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="447" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A447" s="1" t="n">
@@ -19863,6 +21204,9 @@
       <c r="N447" s="1" t="n">
         <v>157.1615721</v>
       </c>
+      <c r="O447" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="448" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A448" s="1" t="n">
@@ -19907,6 +21251,9 @@
       <c r="N448" s="1" t="n">
         <v>173</v>
       </c>
+      <c r="O448" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="449" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A449" s="1" t="n">
@@ -19951,6 +21298,9 @@
       <c r="N449" s="1" t="n">
         <v>178.3171521</v>
       </c>
+      <c r="O449" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="450" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A450" s="1" t="n">
@@ -19995,6 +21345,9 @@
       <c r="N450" s="1" t="n">
         <v>181.0584958</v>
       </c>
+      <c r="O450" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="451" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A451" s="1" t="n">
@@ -20039,6 +21392,9 @@
       <c r="N451" s="1" t="n">
         <v>192.4686192</v>
       </c>
+      <c r="O451" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="452" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A452" s="1" t="n">
@@ -20083,6 +21439,9 @@
       <c r="N452" s="1" t="n">
         <v>167.0360111</v>
       </c>
+      <c r="O452" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="453" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A453" s="1" t="n">
@@ -20127,6 +21486,9 @@
       <c r="N453" s="1" t="n">
         <v>212.3672566</v>
       </c>
+      <c r="O453" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="454" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A454" s="1" t="n">
@@ -20171,6 +21533,9 @@
       <c r="N454" s="1" t="n">
         <v>404.3478261</v>
       </c>
+      <c r="O454" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="455" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A455" s="1" t="n">
@@ -20215,6 +21580,9 @@
       <c r="N455" s="1" t="n">
         <v>239.8373984</v>
       </c>
+      <c r="O455" s="1" t="n">
+        <v>98058</v>
+      </c>
     </row>
     <row r="456" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A456" s="1" t="n">
@@ -20258,6 +21626,9 @@
       </c>
       <c r="N456" s="1" t="n">
         <v>226.0683761</v>
+      </c>
+      <c r="O456" s="1" t="n">
+        <v>98058</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>